<commit_message>
Added numbers to sheets
</commit_message>
<xml_diff>
--- a/Documentation/List of Flexbox Features.xlsx
+++ b/Documentation/List of Flexbox Features.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Data\Demo-projects\Quackathon\FlexBox\StayFlexy\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899A2049-BE40-4999-8BE1-4655F4F5AF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A10A6FB-914A-4331-B9C0-6B7CBCAB679C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33465" yWindow="3045" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Flex Properties To Use" sheetId="2" r:id="rId1"/>
-    <sheet name="Possible Layout" sheetId="3" r:id="rId2"/>
-    <sheet name="Data from MDN" sheetId="1" r:id="rId3"/>
+    <sheet name="(1) Flex Properties To Use" sheetId="2" r:id="rId1"/>
+    <sheet name="(2) Possible Layout" sheetId="3" r:id="rId2"/>
+    <sheet name="(3) Data from MDN" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1934,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3746D3-0A6F-4ABF-AD40-B71DD0CB0FCE}">
   <dimension ref="B2:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,7 +2754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S113"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>